<commit_message>
feta(chart): add some chart
</commit_message>
<xml_diff>
--- a/cluster_list.xlsx
+++ b/cluster_list.xlsx
@@ -576,7 +576,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>410,276,116,100,56,392,757,842,616,268,604,434</t>
+          <t>410,276,116,100,等12项</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -591,12 +591,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>100,276,152,724,710,490,842,699,392,604,36,784,400</t>
+          <t>100,276,152,724,等13项</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>124,826,842,392,642,268,682,376,428,776</t>
+          <t>124,826,842,392,等10项</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -606,7 +606,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>124,528,710,458,36,76,484,490,516,894,699,246,398</t>
+          <t>124,528,710,458,等13项</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -621,27 +621,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>616,381,484,752,975,56,344,251,364,704,458,757,496,268,826,516,180,620,246,76,792,894,192,320,504,51,68,788,70,690,608,40,32,642,804,442,579,764,203,688,512,702,360,418,348,372,188,426,31,376,834,748,703,508,384,837,643,682,408,818,72,454,300,388,92,600,60,214,450,554,591,270,4,838,499,398,860,233,218,417,232,170,598,178,807,762,899,716,586,352,404,478,104,8,275,566,422,24,470,729,208,196,646</t>
+          <t>616,381,484,752,等103项</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>490,516,458,608,381,251,344,894,364,702,764,757,704,300,116,710,320,40,246,566,626,616,792,484,51,512,496,104,643,752,76,688,56,579,540,804,360,70,586,620,528,442,214,188,788,203,192,899,748,180,144,780,662,92,44,585,340,191,705,52,218,348,716,508,426,591,837,384,72,703,634,398,499,31,404,231,504,834,372,690,860,178,729,233,170,598,32,418,68,232,807,450,762,818,470,800,417,466,478,196,8,266,408,454,558,400,414,760,440,12,554</t>
+          <t>490,516,458,608,等111项</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>116,490,458,752,344,616,704,608,381,702,251,364,484,516,56,104,792,246,834,360,764,442,784,170,414,90,320,804,554,496,450,404,788,300,579,528,512,688,642,180,70,12,422,352,40,292,643,682,214,620,586,716,894,508,591,426,837,384,748,203,72,332,92,52,222,703,32,218,566,705,191,348,887,31,8,418,706,196,499,504,398,480,690,440,860,428,729,233,51,598,68,899,232,807,762,417,470,818,288,694,478,340,372,275,178,231,50</t>
+          <t>116,490,458,752,等107项</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>360,826,704,381,792,251,702,344,784,180,376,804,222,752,788,104,404,320,96,608,566,496,364,643,642,40,764,372,688,203,68,620,418,682,32,300,340,440,208,51,352,70,504,384,348,834,508,860,72,31,579,646,818,705,422,499,512,188,84,44,52,586,218,214,408,196,417,899,591,170,598,716,807,8,762,178,706,288,231,478,232,450,568,858,442,262,470,204,577,212,50</t>
+          <t>360,826,704,381,等91项</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>710,458,490,251,826,360,56,688,699,516,344,757,764,100,381,804,704,180,246,320,792,752,800,32,364,218,616,608,116,504,40,579,376,702,642,528,422,643,442,300,784,484,634,404,586,352,620,70,894,384,233,508,499,716,72,418,348,372,454,222,368,533,818,214,682,705,203,554,208,31,690,839,170,51,398,591,232,178,834,899,807,8,68,496,598,566,512,104,748,231,450,144,478,196,762,417,858,440,308,562,568,204,706</t>
+          <t>710,458,490,251,等103项</t>
         </is>
       </c>
     </row>

</xml_diff>